<commit_message>
fix: Update Master Index.xlsx to incorporate recent data modifications
</commit_message>
<xml_diff>
--- a/Master Index.xlsx
+++ b/Master Index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\sortx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C6AA18-7A05-484B-AB4F-774A4B08A5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B291FD9A-D24B-48A0-86E3-BEC5F406824E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UnMapped" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="1476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="1477">
   <si>
     <t>ABK0908-08-E-38-050_03-03</t>
   </si>
@@ -4465,7 +4465,10 @@
     <t>Status</t>
   </si>
   <si>
-    <t>UEsDBBQAAAAIAMd4Ilu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgAx3giW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYAOlKk5n5G9wB6UqTmfkb3AEI1pKZ+RvcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>UEsDBBQAAAAIAOZ4Ilu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgA5ngiW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYAJNpErz5G9wBk2kSvPkb3AEz/wq8+RvcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
   </si>
 </sst>
 </file>
@@ -13115,19 +13118,43 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="3">
+        <v>45902</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D2" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3">
+        <v>45902</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D3" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3">
+        <v>45902</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D4" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -13151,7 +13178,15 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3">
+        <v>45902</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D8" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -13224,7 +13259,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Update Master Index.xlsx with recent data modifications
</commit_message>
<xml_diff>
--- a/Master Index.xlsx
+++ b/Master Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\sortx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE506A5-5F65-4417-9A2D-716386C8113D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E6F698-BF7C-48EA-B736-19802257756A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -726,7 +726,7 @@
     <t>File Name</t>
   </si>
   <si>
-    <t>UEsDBBQAAAAIAKyMIlu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgArIwiW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYAKp6CrcOHNwBqnoKtw4c3AHSaAm3DhzcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
+    <t>UEsDBBQAAAAIAI2NIlu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgAjY0iW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYANNgT7MPHNwB02BPsw8c3AFTnU6zDxzcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1209,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
fix: Update Master Index.xlsx with recent data updates
</commit_message>
<xml_diff>
--- a/Master Index.xlsx
+++ b/Master Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\sortx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E6F698-BF7C-48EA-B736-19802257756A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959B8F4E-5949-45B6-817A-735E976D5AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="ASWXL.Storage" sheetId="5" state="veryHidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="230">
-  <si>
-    <t>Processed Date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="228">
   <si>
     <t>File Path</t>
   </si>
@@ -51,9 +48,6 @@
     <t>C:\Program Files\AspenTech\Aspen Simulation Workbook V14.0</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>P11684-11-01-48-1601-3.pdf</t>
   </si>
   <si>
@@ -726,7 +720,7 @@
     <t>File Name</t>
   </si>
   <si>
-    <t>UEsDBBQAAAAIAI2NIlu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgAjY0iW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYANNgT7MPHNwB02BPsw8c3AFTnU6zDxzcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
+    <t>UEsDBBQAAAAIAAOOIlu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgAA44iW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYAA+2mDYQHNwBD7aYNhAc3AH1pJc2EBzcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
   </si>
 </sst>
 </file>
@@ -771,19 +765,10 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -793,20 +778,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1205,1289 +1185,1143 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D224"/>
+  <dimension ref="A1:B224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="53.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" customWidth="1"/>
-    <col min="4" max="4" width="246.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="246.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="6"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="6"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="6"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="6"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="6"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="5" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="6"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="5" t="s">
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="5" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="6"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="5" t="s">
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="6"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="5" t="s">
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="6"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="5" t="s">
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="5" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="6"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="5" t="s">
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="6"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="5" t="s">
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="6"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="5" t="s">
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="6"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="5" t="s">
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="6"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="5" t="s">
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="6"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="5" t="s">
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="6"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="5" t="s">
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="6"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="5" t="s">
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B58" s="6"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="5" t="s">
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B59" s="6"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="5" t="s">
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B60" s="6"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="5" t="s">
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B61" s="6"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="5" t="s">
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="6"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="5" t="s">
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="6"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="5" t="s">
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="6"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="5" t="s">
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B65" s="6"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" s="5" t="s">
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B66" s="6"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" s="5" t="s">
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B67" s="6"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" s="5" t="s">
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="6"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" s="5" t="s">
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" s="5" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" s="5" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B71" s="6"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" s="5" t="s">
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" s="5" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B73" s="6"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" s="5" t="s">
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B74" s="6"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" s="5" t="s">
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" s="5" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B76" s="6"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" s="5" t="s">
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B77" s="6"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" s="5" t="s">
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B78" s="6"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79" s="5" t="s">
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="6"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80" s="5" t="s">
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B80" s="6"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" s="5" t="s">
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B81" s="6"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" s="5" t="s">
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B82" s="6"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" s="5" t="s">
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B83" s="6"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="5" t="s">
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B84" s="6"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" s="5" t="s">
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B85" s="6"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" s="5" t="s">
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B86" s="6"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" s="5" t="s">
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B87" s="6"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" s="5" t="s">
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" s="5" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" s="5" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" s="5" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B91" s="6"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" s="5" t="s">
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B92" s="6"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" s="5" t="s">
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B93" s="6"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" s="5" t="s">
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B94" s="6"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" s="5" t="s">
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" s="5" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B96" s="6"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" s="5" t="s">
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" s="5" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B98" s="6"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" s="5" t="s">
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B99" s="6"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" s="5" t="s">
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B100" s="6"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" s="5" t="s">
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B101" s="6"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" s="5" t="s">
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" s="5" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" s="5" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" s="5" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B105" s="6"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" s="5" t="s">
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B106" s="6"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" s="5" t="s">
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B107" s="6"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" s="5" t="s">
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B108" s="6"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" s="5" t="s">
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B109" s="6"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" s="5" t="s">
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" s="5" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" s="5" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" s="5" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B113" s="6"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" s="5" t="s">
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B114" s="6"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" s="5" t="s">
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B115" s="6"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" s="5" t="s">
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B116" s="6"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A117" s="5" t="s">
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A118" s="5" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" s="5" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A121" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" s="5" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B120" s="6"/>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" s="5" t="s">
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A123" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B121" s="6"/>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" s="5" t="s">
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A124" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B122" s="6"/>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" s="5" t="s">
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A125" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B123" s="6"/>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" s="5" t="s">
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A126" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" s="5" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A127" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" s="5" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A128" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" s="5" t="s">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A128" s="5" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A130" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B128" s="6"/>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" s="5" t="s">
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" s="5" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" s="5" t="s">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A132" s="5" t="s">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A134" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B132" s="6"/>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A133" s="5" t="s">
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B133" s="6"/>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A134" s="5" t="s">
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A136" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A135" s="5" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A136" s="5" t="s">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A137" s="5" t="s">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A138" s="5" t="s">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A139" s="5" t="s">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A140" s="5" t="s">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B140" s="6"/>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A141" s="5" t="s">
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A143" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B141" s="6"/>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A142" s="5" t="s">
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B142" s="6"/>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A143" s="5" t="s">
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B143" s="6"/>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144" s="5" t="s">
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B144" s="6"/>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" s="5" t="s">
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B145" s="6"/>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A146" s="5" t="s">
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B146" s="6"/>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A147" s="5" t="s">
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A149" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B147" s="6"/>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A148" s="5" t="s">
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A150" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B148" s="6"/>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A149" s="5" t="s">
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B149" s="6"/>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A150" s="5" t="s">
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B150" s="6"/>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A151" s="5" t="s">
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B151" s="6"/>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A152" s="5" t="s">
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B152" s="6"/>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A153" s="5" t="s">
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A155" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A154" s="5" t="s">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A156" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A155" s="5" t="s">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A157" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B155" s="6"/>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A156" s="5" t="s">
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B156" s="6"/>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A157" s="5" t="s">
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A159" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B157" s="6"/>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A158" s="5" t="s">
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B158" s="6"/>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A159" s="5" t="s">
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A160" s="5" t="s">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A161" s="5" t="s">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B161" s="6"/>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A162" s="5" t="s">
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B162" s="6"/>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A163" s="5" t="s">
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B163" s="6"/>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A164" s="5" t="s">
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B164" s="6"/>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A165" s="5" t="s">
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A167" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B165" s="6"/>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A166" s="5" t="s">
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A168" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B166" s="6"/>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A167" s="5" t="s">
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A169" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B167" s="6"/>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A168" s="5" t="s">
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A170" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B168" s="6"/>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A169" s="5" t="s">
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A171" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="B169" s="6"/>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A170" s="5" t="s">
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A172" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A171" s="5" t="s">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A173" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A172" s="5" t="s">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A174" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B172" s="6"/>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A173" s="5" t="s">
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A175" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A174" s="5" t="s">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A176" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B174" s="6"/>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A175" s="5" t="s">
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A177" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A176" s="5" t="s">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A178" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B176" s="6"/>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A177" s="5" t="s">
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A179" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A178" s="5" t="s">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A180" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A179" s="5" t="s">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A181" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B179" s="6"/>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A180" s="5" t="s">
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A182" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B180" s="6"/>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A181" s="5" t="s">
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A183" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A182" s="5" t="s">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A184" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A183" s="5" t="s">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A185" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B183" s="6"/>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A184" s="5" t="s">
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A186" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A185" s="5" t="s">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A187" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B185" s="6"/>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A186" s="5" t="s">
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A188" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B186" s="6"/>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A187" s="5" t="s">
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A189" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A188" s="5" t="s">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A190" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B188" s="6"/>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A189" s="5" t="s">
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A191" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B189" s="6"/>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A190" s="5" t="s">
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A192" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B190" s="6"/>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A191" s="5" t="s">
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A193" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A192" s="5" t="s">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A194" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A193" s="5" t="s">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A195" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B193" s="6"/>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A194" s="5" t="s">
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A196" s="3" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A195" s="5" t="s">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A197" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="B195" s="6"/>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A196" s="5" t="s">
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A198" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A197" s="5" t="s">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A199" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B197" s="6"/>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A198" s="5" t="s">
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A200" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B198" s="6"/>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A199" s="5" t="s">
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A201" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A200" s="5" t="s">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A202" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B200" s="6"/>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A201" s="5" t="s">
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A203" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A202" s="5" t="s">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A204" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A203" s="5" t="s">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A205" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B203" s="6"/>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A204" s="5" t="s">
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A206" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B204" s="6"/>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A205" s="5" t="s">
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A207" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B205" s="6"/>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A206" s="5" t="s">
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A208" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A207" s="5" t="s">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A209" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B207" s="6"/>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A208" s="5" t="s">
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A210" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A209" s="5" t="s">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A211" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A210" s="5" t="s">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A212" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="B210" s="6"/>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A211" s="5" t="s">
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A213" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B211" s="6"/>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A212" s="5" t="s">
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A214" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="B212" s="6"/>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A213" s="5" t="s">
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A215" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A214" s="5" t="s">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A216" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B214" s="6"/>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A215" s="5" t="s">
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A217" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="B215" s="6"/>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A216" s="5" t="s">
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A218" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A217" s="5" t="s">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A219" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A218" s="5" t="s">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A220" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="B218" s="6"/>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A219" s="5" t="s">
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A221" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B219" s="6"/>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A220" s="5" t="s">
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A222" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="B220" s="6"/>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A221" s="5" t="s">
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A223" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A222" s="5" t="s">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A224" s="3" t="s">
         <v>225</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A223" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A224" s="5" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2534,15 +2368,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>229</v>
+      <c r="A2" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>